<commit_message>
add more data bon blanko
</commit_message>
<xml_diff>
--- a/Bon Blanko/Desa Jatimulya/Bon blanko Desa Jatimulya.xlsx
+++ b/Bon Blanko/Desa Jatimulya/Bon blanko Desa Jatimulya.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="241">
   <si>
     <t>No</t>
   </si>
@@ -688,6 +688,57 @@
   </si>
   <si>
     <t>SITI NURJANAH</t>
+  </si>
+  <si>
+    <t>RANI RATNANINGSIH</t>
+  </si>
+  <si>
+    <t>17082/2023</t>
+  </si>
+  <si>
+    <t>MUGIARMAN</t>
+  </si>
+  <si>
+    <t>17160/2023</t>
+  </si>
+  <si>
+    <t>SITI MARDIANI</t>
+  </si>
+  <si>
+    <t>ENUNG MARYAMAH</t>
+  </si>
+  <si>
+    <t>17035/2023</t>
+  </si>
+  <si>
+    <t>DINI LESTARI</t>
+  </si>
+  <si>
+    <t>16979/2023</t>
+  </si>
+  <si>
+    <t>UNDANG SUHERMAN</t>
+  </si>
+  <si>
+    <t>DADI SUPYADI</t>
+  </si>
+  <si>
+    <t>17092/2023</t>
+  </si>
+  <si>
+    <t>EKA FHATHURAHMAN</t>
+  </si>
+  <si>
+    <t>AHMAD HIDAYAT</t>
+  </si>
+  <si>
+    <t>17005/2023</t>
+  </si>
+  <si>
+    <t>TUTI MURNI</t>
+  </si>
+  <si>
+    <t>17089/2023</t>
   </si>
 </sst>
 </file>
@@ -1211,14 +1262,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1561,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,40 +1628,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1636,17 +1687,17 @@
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="6">
-        <v>67983</v>
+      <c r="B6" s="4">
+        <v>61258</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>224</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="E6" s="3">
-        <v>9641</v>
+        <v>9465</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -1654,17 +1705,17 @@
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
-        <v>67984</v>
+      <c r="B7" s="4">
+        <v>61259</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="E7" s="3">
-        <v>9641</v>
+        <v>9465</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1672,17 +1723,17 @@
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="6">
-        <v>67985</v>
+      <c r="B8" s="4">
+        <v>61260</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="E8" s="3">
-        <v>9642</v>
+        <v>9466</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -1690,17 +1741,17 @@
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
-        <v>67986</v>
+      <c r="B9" s="4">
+        <v>61261</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>228</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="E9" s="3">
-        <v>9642</v>
+        <v>9466</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -1708,17 +1759,17 @@
       <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="6">
-        <v>67987</v>
+      <c r="B10" s="4">
+        <v>61262</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="E10" s="3">
-        <v>9643</v>
+        <v>9467</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -1726,17 +1777,17 @@
       <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="6">
-        <v>67988</v>
+      <c r="B11" s="4">
+        <v>61263</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>231</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>232</v>
       </c>
       <c r="E11" s="3">
-        <v>9643</v>
+        <v>9468</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -1744,17 +1795,17 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="6">
-        <v>67989</v>
+      <c r="B12" s="4">
+        <v>61264</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3">
-        <v>9644</v>
+        <v>9469</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -1762,17 +1813,17 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="6">
-        <v>67990</v>
+      <c r="B13" s="4">
+        <v>61265</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>235</v>
       </c>
       <c r="E13" s="3">
-        <v>9644</v>
+        <v>9470</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -1780,17 +1831,17 @@
       <c r="A14" s="2">
         <v>9</v>
       </c>
-      <c r="B14" s="6">
-        <v>67991</v>
+      <c r="B14" s="4">
+        <v>61266</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E14" s="3">
-        <v>9678</v>
+        <v>9471</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -1798,17 +1849,17 @@
       <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B15" s="6">
-        <v>67992</v>
+      <c r="B15" s="4">
+        <v>61268</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>238</v>
       </c>
       <c r="E15" s="3">
-        <v>9678</v>
+        <v>9472</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -1816,17 +1867,17 @@
       <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="B16" s="6">
-        <v>67993</v>
+      <c r="B16" s="4">
+        <v>61368</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>239</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
+        <v>240</v>
       </c>
       <c r="E16" s="3">
-        <v>9678</v>
+        <v>9473</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -1834,17 +1885,17 @@
       <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="B17" s="6">
-        <v>67994</v>
+      <c r="B17" s="4">
+        <v>67983</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3">
-        <v>9679</v>
+        <v>9641</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -1852,17 +1903,17 @@
       <c r="A18" s="2">
         <v>13</v>
       </c>
-      <c r="B18" s="6">
-        <v>67995</v>
+      <c r="B18" s="4">
+        <v>67984</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3">
-        <v>9679</v>
+        <v>9641</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -1870,17 +1921,17 @@
       <c r="A19" s="2">
         <v>14</v>
       </c>
-      <c r="B19" s="6">
-        <v>68009</v>
+      <c r="B19" s="4">
+        <v>67985</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E19" s="3">
-        <v>9691</v>
+        <v>9642</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -1888,17 +1939,17 @@
       <c r="A20" s="2">
         <v>15</v>
       </c>
-      <c r="B20" s="6">
-        <v>68010</v>
+      <c r="B20" s="4">
+        <v>67986</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E20" s="3">
-        <v>9692</v>
+        <v>9642</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -1906,17 +1957,17 @@
       <c r="A21" s="2">
         <v>16</v>
       </c>
-      <c r="B21" s="6">
-        <v>68011</v>
+      <c r="B21" s="4">
+        <v>67987</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E21" s="3">
-        <v>9693</v>
+        <v>9643</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -1924,17 +1975,17 @@
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="6">
-        <v>76683</v>
+      <c r="B22" s="4">
+        <v>67988</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E22" s="3">
-        <v>10123</v>
+        <v>9643</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -1942,17 +1993,17 @@
       <c r="A23" s="2">
         <v>18</v>
       </c>
-      <c r="B23" s="6">
-        <v>76684</v>
+      <c r="B23" s="4">
+        <v>67989</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3">
-        <v>10124</v>
+        <v>9644</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -1960,17 +2011,17 @@
       <c r="A24" s="2">
         <v>19</v>
       </c>
-      <c r="B24" s="6">
-        <v>76685</v>
+      <c r="B24" s="4">
+        <v>67990</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E24" s="3">
-        <v>10125</v>
+        <v>9644</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -1978,17 +2029,17 @@
       <c r="A25" s="2">
         <v>20</v>
       </c>
-      <c r="B25" s="6">
-        <v>76686</v>
+      <c r="B25" s="4">
+        <v>67991</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E25" s="3">
-        <v>10126</v>
+        <v>9678</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -1996,17 +2047,17 @@
       <c r="A26" s="2">
         <v>21</v>
       </c>
-      <c r="B26" s="6">
-        <v>76688</v>
+      <c r="B26" s="4">
+        <v>67992</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E26" s="3">
-        <v>10127</v>
+        <v>9678</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -2014,17 +2065,17 @@
       <c r="A27" s="2">
         <v>22</v>
       </c>
-      <c r="B27" s="6">
-        <v>76689</v>
+      <c r="B27" s="4">
+        <v>67993</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="E27" s="3">
-        <v>10128</v>
+        <v>9678</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -2032,17 +2083,17 @@
       <c r="A28" s="2">
         <v>23</v>
       </c>
-      <c r="B28" s="3">
-        <v>76692</v>
+      <c r="B28" s="4">
+        <v>67994</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3">
-        <v>13893</v>
+        <v>9679</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2050,17 +2101,17 @@
       <c r="A29" s="2">
         <v>24</v>
       </c>
-      <c r="B29" s="2">
-        <v>76694</v>
+      <c r="B29" s="4">
+        <v>67995</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E29" s="3">
-        <v>13894</v>
+        <v>9679</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -2068,17 +2119,17 @@
       <c r="A30" s="2">
         <v>25</v>
       </c>
-      <c r="B30" s="3">
-        <v>76695</v>
+      <c r="B30" s="4">
+        <v>68009</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E30" s="3">
-        <v>13893</v>
+        <v>9691</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -2086,17 +2137,17 @@
       <c r="A31" s="2">
         <v>26</v>
       </c>
-      <c r="B31" s="3">
-        <v>76697</v>
+      <c r="B31" s="4">
+        <v>68010</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3">
-        <v>13895</v>
+        <v>9692</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -2104,17 +2155,17 @@
       <c r="A32" s="2">
         <v>27</v>
       </c>
-      <c r="B32" s="3">
-        <v>76698</v>
+      <c r="B32" s="4">
+        <v>68011</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3">
-        <v>13895</v>
+        <v>9693</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -2122,17 +2173,17 @@
       <c r="A33" s="2">
         <v>28</v>
       </c>
-      <c r="B33" s="3">
-        <v>76700</v>
+      <c r="B33" s="4">
+        <v>76683</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E33" s="3">
-        <v>13895</v>
+        <v>10123</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -2140,17 +2191,17 @@
       <c r="A34" s="2">
         <v>29</v>
       </c>
-      <c r="B34" s="3">
-        <v>76701</v>
+      <c r="B34" s="4">
+        <v>76684</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E34" s="3">
-        <v>13895</v>
+        <v>10124</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -2158,17 +2209,17 @@
       <c r="A35" s="2">
         <v>30</v>
       </c>
-      <c r="B35" s="3">
-        <v>76702</v>
+      <c r="B35" s="4">
+        <v>76685</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3">
-        <v>13895</v>
+        <v>10125</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2176,17 +2227,17 @@
       <c r="A36" s="2">
         <v>31</v>
       </c>
-      <c r="B36" s="3">
-        <v>76704</v>
+      <c r="B36" s="4">
+        <v>76686</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E36" s="3">
-        <v>13895</v>
+        <v>10126</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -2194,17 +2245,17 @@
       <c r="A37" s="2">
         <v>32</v>
       </c>
-      <c r="B37" s="3">
-        <v>76706</v>
+      <c r="B37" s="4">
+        <v>76688</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E37" s="3">
-        <v>13895</v>
+        <v>10127</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -2212,17 +2263,17 @@
       <c r="A38" s="2">
         <v>33</v>
       </c>
-      <c r="B38" s="2">
-        <v>76707</v>
+      <c r="B38" s="4">
+        <v>76689</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E38" s="3">
-        <v>13894</v>
+        <v>10128</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -2230,17 +2281,17 @@
       <c r="A39" s="2">
         <v>34</v>
       </c>
-      <c r="B39" s="2">
-        <v>76709</v>
+      <c r="B39" s="3">
+        <v>76692</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E39" s="3">
-        <v>13894</v>
+        <v>13893</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -2248,17 +2299,17 @@
       <c r="A40" s="2">
         <v>35</v>
       </c>
-      <c r="B40" s="3">
-        <v>76711</v>
+      <c r="B40" s="2">
+        <v>76694</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E40" s="3">
-        <v>13896</v>
+        <v>13894</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -2266,17 +2317,17 @@
       <c r="A41" s="2">
         <v>36</v>
       </c>
-      <c r="B41" s="2">
-        <v>76712</v>
+      <c r="B41" s="3">
+        <v>76695</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E41" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -2285,10 +2336,10 @@
         <v>37</v>
       </c>
       <c r="B42" s="3">
-        <v>76714</v>
+        <v>76697</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>46</v>
@@ -2302,17 +2353,17 @@
       <c r="A43" s="2">
         <v>38</v>
       </c>
-      <c r="B43" s="6">
-        <v>76715</v>
+      <c r="B43" s="3">
+        <v>76698</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E43" s="3">
-        <v>14184</v>
+        <v>13895</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -2320,17 +2371,17 @@
       <c r="A44" s="2">
         <v>39</v>
       </c>
-      <c r="B44" s="6">
-        <v>76719</v>
+      <c r="B44" s="3">
+        <v>76700</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E44" s="3">
-        <v>13897</v>
+        <v>13895</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -2338,17 +2389,17 @@
       <c r="A45" s="2">
         <v>40</v>
       </c>
-      <c r="B45" s="6">
-        <v>76720</v>
+      <c r="B45" s="3">
+        <v>76701</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E45" s="3">
-        <v>13897</v>
+        <v>13895</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -2356,17 +2407,17 @@
       <c r="A46" s="2">
         <v>41</v>
       </c>
-      <c r="B46" s="2">
-        <v>76722</v>
+      <c r="B46" s="3">
+        <v>76702</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E46" s="3">
-        <v>13894</v>
+        <v>13895</v>
       </c>
       <c r="F46" s="3"/>
     </row>
@@ -2374,17 +2425,17 @@
       <c r="A47" s="2">
         <v>42</v>
       </c>
-      <c r="B47" s="2">
-        <v>76723</v>
+      <c r="B47" s="3">
+        <v>76704</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E47" s="3">
-        <v>13894</v>
+        <v>13895</v>
       </c>
       <c r="F47" s="3"/>
     </row>
@@ -2392,17 +2443,17 @@
       <c r="A48" s="2">
         <v>43</v>
       </c>
-      <c r="B48" s="6">
-        <v>76724</v>
+      <c r="B48" s="3">
+        <v>76706</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E48" s="3">
-        <v>13898</v>
+        <v>13895</v>
       </c>
       <c r="F48" s="3"/>
     </row>
@@ -2410,17 +2461,17 @@
       <c r="A49" s="2">
         <v>44</v>
       </c>
-      <c r="B49" s="6">
-        <v>76725</v>
+      <c r="B49" s="2">
+        <v>76707</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E49" s="3">
-        <v>13898</v>
+        <v>13894</v>
       </c>
       <c r="F49" s="3"/>
     </row>
@@ -2428,17 +2479,17 @@
       <c r="A50" s="2">
         <v>45</v>
       </c>
-      <c r="B50" s="6">
-        <v>76726</v>
+      <c r="B50" s="2">
+        <v>76709</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E50" s="3">
-        <v>13899</v>
+        <v>13894</v>
       </c>
       <c r="F50" s="3"/>
     </row>
@@ -2446,17 +2497,17 @@
       <c r="A51" s="2">
         <v>46</v>
       </c>
-      <c r="B51" s="6">
-        <v>76728</v>
+      <c r="B51" s="3">
+        <v>76711</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E51" s="3">
-        <v>13899</v>
+        <v>13896</v>
       </c>
       <c r="F51" s="3"/>
     </row>
@@ -2464,17 +2515,17 @@
       <c r="A52" s="2">
         <v>47</v>
       </c>
-      <c r="B52" s="6">
-        <v>76730</v>
+      <c r="B52" s="2">
+        <v>76712</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E52" s="3">
-        <v>13900</v>
+        <v>13896</v>
       </c>
       <c r="F52" s="3"/>
     </row>
@@ -2483,16 +2534,16 @@
         <v>48</v>
       </c>
       <c r="B53" s="3">
-        <v>76732</v>
+        <v>76714</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E53" s="3">
-        <v>13900</v>
+        <v>13895</v>
       </c>
       <c r="F53" s="3"/>
     </row>
@@ -2500,17 +2551,17 @@
       <c r="A54" s="2">
         <v>49</v>
       </c>
-      <c r="B54" s="3">
-        <v>76733</v>
+      <c r="B54" s="4">
+        <v>76715</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3">
-        <v>13900</v>
+        <v>14184</v>
       </c>
       <c r="F54" s="3"/>
     </row>
@@ -2518,17 +2569,17 @@
       <c r="A55" s="2">
         <v>50</v>
       </c>
-      <c r="B55" s="3">
-        <v>76735</v>
+      <c r="B55" s="4">
+        <v>76719</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E55" s="3">
-        <v>13900</v>
+        <v>13897</v>
       </c>
       <c r="F55" s="3"/>
     </row>
@@ -2536,17 +2587,17 @@
       <c r="A56" s="2">
         <v>51</v>
       </c>
-      <c r="B56" s="6">
-        <v>76736</v>
+      <c r="B56" s="4">
+        <v>76720</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E56" s="3">
-        <v>13900</v>
+        <v>13897</v>
       </c>
       <c r="F56" s="3"/>
     </row>
@@ -2554,17 +2605,17 @@
       <c r="A57" s="2">
         <v>52</v>
       </c>
-      <c r="B57" s="6">
-        <v>76739</v>
+      <c r="B57" s="2">
+        <v>76722</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E57" s="3">
-        <v>13900</v>
+        <v>13894</v>
       </c>
       <c r="F57" s="3"/>
     </row>
@@ -2572,17 +2623,17 @@
       <c r="A58" s="2">
         <v>53</v>
       </c>
-      <c r="B58" s="6">
-        <v>76740</v>
+      <c r="B58" s="2">
+        <v>76723</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E58" s="3">
-        <v>13900</v>
+        <v>13894</v>
       </c>
       <c r="F58" s="3"/>
     </row>
@@ -2590,17 +2641,17 @@
       <c r="A59" s="2">
         <v>54</v>
       </c>
-      <c r="B59" s="6">
-        <v>76741</v>
+      <c r="B59" s="4">
+        <v>76724</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E59" s="3">
-        <v>13901</v>
+        <v>13898</v>
       </c>
       <c r="F59" s="3"/>
     </row>
@@ -2608,17 +2659,17 @@
       <c r="A60" s="2">
         <v>55</v>
       </c>
-      <c r="B60" s="2">
-        <v>76742</v>
+      <c r="B60" s="4">
+        <v>76725</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E60" s="3">
-        <v>13896</v>
+        <v>13898</v>
       </c>
       <c r="F60" s="3"/>
     </row>
@@ -2626,17 +2677,17 @@
       <c r="A61" s="2">
         <v>56</v>
       </c>
-      <c r="B61" s="6">
-        <v>76743</v>
+      <c r="B61" s="4">
+        <v>76726</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E61" s="3">
-        <v>13898</v>
+        <v>13899</v>
       </c>
       <c r="F61" s="3"/>
     </row>
@@ -2644,17 +2695,17 @@
       <c r="A62" s="2">
         <v>57</v>
       </c>
-      <c r="B62" s="3">
-        <v>76744</v>
+      <c r="B62" s="4">
+        <v>76728</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="E62" s="3">
-        <v>13895</v>
+        <v>13899</v>
       </c>
       <c r="F62" s="3"/>
     </row>
@@ -2662,17 +2713,17 @@
       <c r="A63" s="2">
         <v>58</v>
       </c>
-      <c r="B63" s="2">
-        <v>76746</v>
+      <c r="B63" s="4">
+        <v>76730</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="E63" s="3">
-        <v>13895</v>
+        <v>13900</v>
       </c>
       <c r="F63" s="3"/>
     </row>
@@ -2681,16 +2732,16 @@
         <v>59</v>
       </c>
       <c r="B64" s="3">
-        <v>76747</v>
+        <v>76732</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E64" s="3">
-        <v>13902</v>
+        <v>13900</v>
       </c>
       <c r="F64" s="3"/>
     </row>
@@ -2698,17 +2749,17 @@
       <c r="A65" s="2">
         <v>60</v>
       </c>
-      <c r="B65" s="6">
-        <v>76749</v>
+      <c r="B65" s="3">
+        <v>76733</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E65" s="3">
-        <v>13899</v>
+        <v>13900</v>
       </c>
       <c r="F65" s="3"/>
     </row>
@@ -2716,17 +2767,17 @@
       <c r="A66" s="2">
         <v>61</v>
       </c>
-      <c r="B66" s="6">
-        <v>76750</v>
+      <c r="B66" s="3">
+        <v>76735</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E66" s="3">
-        <v>13902</v>
+        <v>13900</v>
       </c>
       <c r="F66" s="3"/>
     </row>
@@ -2734,17 +2785,17 @@
       <c r="A67" s="2">
         <v>62</v>
       </c>
-      <c r="B67" s="6">
-        <v>76752</v>
+      <c r="B67" s="4">
+        <v>76736</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E67" s="3">
-        <v>13902</v>
+        <v>13900</v>
       </c>
       <c r="F67" s="3"/>
     </row>
@@ -2752,17 +2803,17 @@
       <c r="A68" s="2">
         <v>63</v>
       </c>
-      <c r="B68" s="3">
-        <v>76753</v>
+      <c r="B68" s="4">
+        <v>76739</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E68" s="3">
-        <v>13901</v>
+        <v>13900</v>
       </c>
       <c r="F68" s="3"/>
     </row>
@@ -2770,17 +2821,17 @@
       <c r="A69" s="2">
         <v>64</v>
       </c>
-      <c r="B69" s="6">
-        <v>76757</v>
+      <c r="B69" s="4">
+        <v>76740</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E69" s="3">
-        <v>13898</v>
+        <v>13900</v>
       </c>
       <c r="F69" s="3"/>
     </row>
@@ -2788,17 +2839,17 @@
       <c r="A70" s="2">
         <v>65</v>
       </c>
-      <c r="B70" s="6">
-        <v>76758</v>
+      <c r="B70" s="4">
+        <v>76741</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E70" s="3">
-        <v>13899</v>
+        <v>13901</v>
       </c>
       <c r="F70" s="3"/>
     </row>
@@ -2806,17 +2857,17 @@
       <c r="A71" s="2">
         <v>66</v>
       </c>
-      <c r="B71" s="6">
-        <v>76762</v>
+      <c r="B71" s="2">
+        <v>76742</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="E71" s="3">
-        <v>10129</v>
+        <v>13896</v>
       </c>
       <c r="F71" s="3"/>
     </row>
@@ -2824,17 +2875,17 @@
       <c r="A72" s="2">
         <v>67</v>
       </c>
-      <c r="B72" s="6">
-        <v>76764</v>
+      <c r="B72" s="4">
+        <v>76743</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E72" s="3">
-        <v>10130</v>
+        <v>13898</v>
       </c>
       <c r="F72" s="3"/>
     </row>
@@ -2842,17 +2893,17 @@
       <c r="A73" s="2">
         <v>68</v>
       </c>
-      <c r="B73" s="6">
-        <v>76765</v>
+      <c r="B73" s="3">
+        <v>76744</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E73" s="3">
-        <v>10131</v>
+        <v>13895</v>
       </c>
       <c r="F73" s="3"/>
     </row>
@@ -2860,17 +2911,17 @@
       <c r="A74" s="2">
         <v>69</v>
       </c>
-      <c r="B74" s="6">
-        <v>76766</v>
+      <c r="B74" s="2">
+        <v>76746</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="E74" s="3">
-        <v>10132</v>
+        <v>13895</v>
       </c>
       <c r="F74" s="3"/>
     </row>
@@ -2878,17 +2929,17 @@
       <c r="A75" s="2">
         <v>70</v>
       </c>
-      <c r="B75" s="6">
-        <v>76767</v>
+      <c r="B75" s="3">
+        <v>76747</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E75" s="3">
-        <v>10133</v>
+        <v>13902</v>
       </c>
       <c r="F75" s="3"/>
     </row>
@@ -2896,17 +2947,17 @@
       <c r="A76" s="2">
         <v>71</v>
       </c>
-      <c r="B76" s="6">
-        <v>76769</v>
+      <c r="B76" s="4">
+        <v>76749</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E76" s="3">
-        <v>10134</v>
+        <v>13899</v>
       </c>
       <c r="F76" s="3"/>
     </row>
@@ -2914,17 +2965,17 @@
       <c r="A77" s="2">
         <v>72</v>
       </c>
-      <c r="B77" s="6">
-        <v>76771</v>
+      <c r="B77" s="4">
+        <v>76750</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E77" s="3">
-        <v>10135</v>
+        <v>13902</v>
       </c>
       <c r="F77" s="3"/>
     </row>
@@ -2932,17 +2983,17 @@
       <c r="A78" s="2">
         <v>73</v>
       </c>
-      <c r="B78" s="2">
-        <v>76772</v>
+      <c r="B78" s="4">
+        <v>76752</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E78" s="3">
-        <v>12582</v>
+        <v>13902</v>
       </c>
       <c r="F78" s="3"/>
     </row>
@@ -2950,17 +3001,17 @@
       <c r="A79" s="2">
         <v>74</v>
       </c>
-      <c r="B79" s="6">
-        <v>76774</v>
+      <c r="B79" s="3">
+        <v>76753</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E79" s="3">
-        <v>10136</v>
+        <v>13901</v>
       </c>
       <c r="F79" s="3"/>
     </row>
@@ -2968,17 +3019,17 @@
       <c r="A80" s="2">
         <v>75</v>
       </c>
-      <c r="B80" s="6">
-        <v>76776</v>
+      <c r="B80" s="4">
+        <v>76757</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="E80" s="3">
-        <v>12582</v>
+        <v>13898</v>
       </c>
       <c r="F80" s="3"/>
     </row>
@@ -2986,17 +3037,17 @@
       <c r="A81" s="2">
         <v>76</v>
       </c>
-      <c r="B81" s="6">
-        <v>76777</v>
+      <c r="B81" s="4">
+        <v>76758</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="E81" s="3">
-        <v>10138</v>
+        <v>13899</v>
       </c>
       <c r="F81" s="3"/>
     </row>
@@ -3004,17 +3055,17 @@
       <c r="A82" s="2">
         <v>77</v>
       </c>
-      <c r="B82" s="6">
-        <v>76780</v>
+      <c r="B82" s="4">
+        <v>76762</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E82" s="3">
-        <v>10139</v>
+        <v>10129</v>
       </c>
       <c r="F82" s="3"/>
     </row>
@@ -3022,17 +3073,17 @@
       <c r="A83" s="2">
         <v>78</v>
       </c>
-      <c r="B83" s="6">
-        <v>76781</v>
+      <c r="B83" s="4">
+        <v>76764</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="E83" s="3">
-        <v>10140</v>
+        <v>10130</v>
       </c>
       <c r="F83" s="3"/>
     </row>
@@ -3040,17 +3091,17 @@
       <c r="A84" s="2">
         <v>79</v>
       </c>
-      <c r="B84" s="6">
-        <v>76783</v>
+      <c r="B84" s="4">
+        <v>76765</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E84" s="3">
-        <v>10141</v>
+        <v>10131</v>
       </c>
       <c r="F84" s="3"/>
     </row>
@@ -3058,17 +3109,17 @@
       <c r="A85" s="2">
         <v>80</v>
       </c>
-      <c r="B85" s="6">
-        <v>76784</v>
+      <c r="B85" s="4">
+        <v>76766</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="E85" s="3">
-        <v>10141</v>
+        <v>10132</v>
       </c>
       <c r="F85" s="3"/>
     </row>
@@ -3076,17 +3127,17 @@
       <c r="A86" s="2">
         <v>81</v>
       </c>
-      <c r="B86" s="6">
-        <v>76787</v>
+      <c r="B86" s="4">
+        <v>76767</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E86" s="3">
-        <v>10141</v>
+        <v>10133</v>
       </c>
       <c r="F86" s="3"/>
     </row>
@@ -3094,17 +3145,17 @@
       <c r="A87" s="2">
         <v>82</v>
       </c>
-      <c r="B87" s="6">
-        <v>76788</v>
+      <c r="B87" s="4">
+        <v>76769</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E87" s="3">
-        <v>10141</v>
+        <v>10134</v>
       </c>
       <c r="F87" s="3"/>
     </row>
@@ -3112,17 +3163,17 @@
       <c r="A88" s="2">
         <v>83</v>
       </c>
-      <c r="B88" s="6">
-        <v>76789</v>
+      <c r="B88" s="4">
+        <v>76771</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E88" s="3">
-        <v>10142</v>
+        <v>10135</v>
       </c>
       <c r="F88" s="3"/>
     </row>
@@ -3130,17 +3181,17 @@
       <c r="A89" s="2">
         <v>84</v>
       </c>
-      <c r="B89" s="6">
-        <v>76790</v>
+      <c r="B89" s="2">
+        <v>76772</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E89" s="3">
-        <v>10142</v>
+        <v>12582</v>
       </c>
       <c r="F89" s="3"/>
     </row>
@@ -3148,17 +3199,17 @@
       <c r="A90" s="2">
         <v>85</v>
       </c>
-      <c r="B90" s="6">
-        <v>76791</v>
+      <c r="B90" s="4">
+        <v>76774</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E90" s="3">
-        <v>10143</v>
+        <v>10136</v>
       </c>
       <c r="F90" s="3"/>
     </row>
@@ -3166,17 +3217,17 @@
       <c r="A91" s="2">
         <v>86</v>
       </c>
-      <c r="B91" s="6">
-        <v>76792</v>
+      <c r="B91" s="4">
+        <v>76776</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E91" s="3">
-        <v>10144</v>
+        <v>12582</v>
       </c>
       <c r="F91" s="3"/>
     </row>
@@ -3184,17 +3235,17 @@
       <c r="A92" s="2">
         <v>87</v>
       </c>
-      <c r="B92" s="6">
-        <v>76794</v>
+      <c r="B92" s="4">
+        <v>76777</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E92" s="3">
-        <v>10145</v>
+        <v>10138</v>
       </c>
       <c r="F92" s="3"/>
     </row>
@@ -3202,17 +3253,17 @@
       <c r="A93" s="2">
         <v>88</v>
       </c>
-      <c r="B93" s="6">
-        <v>76795</v>
+      <c r="B93" s="4">
+        <v>76780</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E93" s="3">
-        <v>10145</v>
+        <v>10139</v>
       </c>
       <c r="F93" s="3"/>
     </row>
@@ -3220,17 +3271,17 @@
       <c r="A94" s="2">
         <v>89</v>
       </c>
-      <c r="B94" s="6">
-        <v>76797</v>
+      <c r="B94" s="4">
+        <v>76781</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>130</v>
+        <v>47</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E94" s="3">
-        <v>10146</v>
+        <v>10140</v>
       </c>
       <c r="F94" s="3"/>
     </row>
@@ -3238,17 +3289,17 @@
       <c r="A95" s="2">
         <v>90</v>
       </c>
-      <c r="B95" s="6">
-        <v>76799</v>
+      <c r="B95" s="4">
+        <v>76783</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="E95" s="3">
-        <v>10147</v>
+        <v>10141</v>
       </c>
       <c r="F95" s="3"/>
     </row>
@@ -3256,17 +3307,17 @@
       <c r="A96" s="2">
         <v>91</v>
       </c>
-      <c r="B96" s="6">
-        <v>76801</v>
+      <c r="B96" s="4">
+        <v>76784</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E96" s="3">
-        <v>10148</v>
+        <v>10141</v>
       </c>
       <c r="F96" s="3"/>
     </row>
@@ -3274,17 +3325,17 @@
       <c r="A97" s="2">
         <v>92</v>
       </c>
-      <c r="B97" s="6">
-        <v>76802</v>
+      <c r="B97" s="4">
+        <v>76787</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E97" s="3">
-        <v>10149</v>
+        <v>10141</v>
       </c>
       <c r="F97" s="3"/>
     </row>
@@ -3292,17 +3343,17 @@
       <c r="A98" s="2">
         <v>93</v>
       </c>
-      <c r="B98" s="6">
-        <v>76804</v>
+      <c r="B98" s="4">
+        <v>76788</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E98" s="3">
-        <v>10149</v>
+        <v>10141</v>
       </c>
       <c r="F98" s="3"/>
     </row>
@@ -3310,17 +3361,17 @@
       <c r="A99" s="2">
         <v>94</v>
       </c>
-      <c r="B99" s="6">
-        <v>76806</v>
+      <c r="B99" s="4">
+        <v>76789</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="E99" s="3">
-        <v>10150</v>
+        <v>10142</v>
       </c>
       <c r="F99" s="3"/>
     </row>
@@ -3328,17 +3379,17 @@
       <c r="A100" s="2">
         <v>95</v>
       </c>
-      <c r="B100" s="6">
-        <v>76808</v>
+      <c r="B100" s="4">
+        <v>76790</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E100" s="3">
-        <v>10151</v>
+        <v>10142</v>
       </c>
       <c r="F100" s="3"/>
     </row>
@@ -3346,17 +3397,17 @@
       <c r="A101" s="2">
         <v>96</v>
       </c>
-      <c r="B101" s="6">
-        <v>76810</v>
+      <c r="B101" s="4">
+        <v>76791</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E101" s="3">
-        <v>10152</v>
+        <v>10143</v>
       </c>
       <c r="F101" s="3"/>
     </row>
@@ -3364,17 +3415,17 @@
       <c r="A102" s="2">
         <v>97</v>
       </c>
-      <c r="B102" s="6">
-        <v>76811</v>
+      <c r="B102" s="4">
+        <v>76792</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E102" s="3">
-        <v>10153</v>
+        <v>10144</v>
       </c>
       <c r="F102" s="3"/>
     </row>
@@ -3382,17 +3433,17 @@
       <c r="A103" s="2">
         <v>98</v>
       </c>
-      <c r="B103" s="6">
-        <v>76812</v>
+      <c r="B103" s="4">
+        <v>76794</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E103" s="3">
-        <v>10153</v>
+        <v>10145</v>
       </c>
       <c r="F103" s="3"/>
     </row>
@@ -3400,17 +3451,17 @@
       <c r="A104" s="2">
         <v>99</v>
       </c>
-      <c r="B104" s="2">
-        <v>77714</v>
+      <c r="B104" s="4">
+        <v>76795</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="E104" s="3">
-        <v>12583</v>
+        <v>10145</v>
       </c>
       <c r="F104" s="3"/>
     </row>
@@ -3418,17 +3469,17 @@
       <c r="A105" s="2">
         <v>100</v>
       </c>
-      <c r="B105" s="2">
-        <v>77720</v>
+      <c r="B105" s="4">
+        <v>76797</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E105" s="3">
-        <v>12584</v>
+        <v>10146</v>
       </c>
       <c r="F105" s="3"/>
     </row>
@@ -3436,17 +3487,17 @@
       <c r="A106" s="2">
         <v>101</v>
       </c>
-      <c r="B106" s="2">
-        <v>77721</v>
+      <c r="B106" s="4">
+        <v>76799</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E106" s="3">
-        <v>12585</v>
+        <v>10147</v>
       </c>
       <c r="F106" s="3"/>
     </row>
@@ -3454,17 +3505,17 @@
       <c r="A107" s="2">
         <v>102</v>
       </c>
-      <c r="B107" s="6">
-        <v>77731</v>
+      <c r="B107" s="4">
+        <v>76801</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E107" s="3">
-        <v>10992</v>
+        <v>10148</v>
       </c>
       <c r="F107" s="3"/>
     </row>
@@ -3472,17 +3523,17 @@
       <c r="A108" s="2">
         <v>103</v>
       </c>
-      <c r="B108" s="2">
-        <v>77734</v>
+      <c r="B108" s="4">
+        <v>76802</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="E108" s="3">
-        <v>12586</v>
+        <v>10149</v>
       </c>
       <c r="F108" s="3"/>
     </row>
@@ -3490,17 +3541,17 @@
       <c r="A109" s="2">
         <v>104</v>
       </c>
-      <c r="B109" s="2">
-        <v>77738</v>
+      <c r="B109" s="4">
+        <v>76804</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="E109" s="3">
-        <v>12587</v>
+        <v>10149</v>
       </c>
       <c r="F109" s="3"/>
     </row>
@@ -3508,17 +3559,17 @@
       <c r="A110" s="2">
         <v>105</v>
       </c>
-      <c r="B110" s="3">
-        <v>77756</v>
+      <c r="B110" s="4">
+        <v>76806</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="E110" s="3">
-        <v>13893</v>
+        <v>10150</v>
       </c>
       <c r="F110" s="3"/>
     </row>
@@ -3526,17 +3577,17 @@
       <c r="A111" s="2">
         <v>106</v>
       </c>
-      <c r="B111" s="3">
-        <v>77760</v>
+      <c r="B111" s="4">
+        <v>76808</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="E111" s="3">
-        <v>13893</v>
+        <v>10151</v>
       </c>
       <c r="F111" s="3"/>
     </row>
@@ -3544,17 +3595,17 @@
       <c r="A112" s="2">
         <v>107</v>
       </c>
-      <c r="B112" s="3">
-        <v>77761</v>
+      <c r="B112" s="4">
+        <v>76810</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="E112" s="3">
-        <v>13893</v>
+        <v>10152</v>
       </c>
       <c r="F112" s="3"/>
     </row>
@@ -3562,17 +3613,17 @@
       <c r="A113" s="2">
         <v>108</v>
       </c>
-      <c r="B113" s="3">
-        <v>77766</v>
+      <c r="B113" s="4">
+        <v>76811</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="E113" s="3">
-        <v>13893</v>
+        <v>10153</v>
       </c>
       <c r="F113" s="3"/>
     </row>
@@ -3580,17 +3631,17 @@
       <c r="A114" s="2">
         <v>109</v>
       </c>
-      <c r="B114" s="3">
-        <v>77770</v>
+      <c r="B114" s="4">
+        <v>76812</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="E114" s="3">
-        <v>13893</v>
+        <v>10153</v>
       </c>
       <c r="F114" s="3"/>
     </row>
@@ -3598,17 +3649,17 @@
       <c r="A115" s="2">
         <v>110</v>
       </c>
-      <c r="B115" s="3">
-        <v>77777</v>
+      <c r="B115" s="2">
+        <v>77714</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E115" s="3">
-        <v>13893</v>
+        <v>12583</v>
       </c>
       <c r="F115" s="3"/>
     </row>
@@ -3616,17 +3667,17 @@
       <c r="A116" s="2">
         <v>111</v>
       </c>
-      <c r="B116" s="3">
-        <v>77778</v>
+      <c r="B116" s="2">
+        <v>77720</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="E116" s="3">
-        <v>13896</v>
+        <v>12584</v>
       </c>
       <c r="F116" s="3"/>
     </row>
@@ -3634,17 +3685,17 @@
       <c r="A117" s="2">
         <v>112</v>
       </c>
-      <c r="B117" s="3">
-        <v>77780</v>
+      <c r="B117" s="2">
+        <v>77721</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="E117" s="3">
-        <v>13896</v>
+        <v>12585</v>
       </c>
       <c r="F117" s="3"/>
     </row>
@@ -3652,17 +3703,17 @@
       <c r="A118" s="2">
         <v>113</v>
       </c>
-      <c r="B118" s="3">
-        <v>77781</v>
+      <c r="B118" s="4">
+        <v>77731</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="E118" s="3">
-        <v>13896</v>
+        <v>10992</v>
       </c>
       <c r="F118" s="3"/>
     </row>
@@ -3670,17 +3721,17 @@
       <c r="A119" s="2">
         <v>114</v>
       </c>
-      <c r="B119" s="3">
-        <v>77782</v>
+      <c r="B119" s="2">
+        <v>77734</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="E119" s="3">
-        <v>13896</v>
+        <v>12586</v>
       </c>
       <c r="F119" s="3"/>
     </row>
@@ -3688,17 +3739,17 @@
       <c r="A120" s="2">
         <v>115</v>
       </c>
-      <c r="B120" s="3">
-        <v>77834</v>
+      <c r="B120" s="2">
+        <v>77738</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E120" s="3">
-        <v>13896</v>
+        <v>12587</v>
       </c>
       <c r="F120" s="3"/>
     </row>
@@ -3706,17 +3757,17 @@
       <c r="A121" s="2">
         <v>116</v>
       </c>
-      <c r="B121" s="6">
-        <v>77835</v>
+      <c r="B121" s="3">
+        <v>77756</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E121" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F121" s="3"/>
     </row>
@@ -3725,16 +3776,16 @@
         <v>117</v>
       </c>
       <c r="B122" s="3">
-        <v>77836</v>
+        <v>77760</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E122" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F122" s="3"/>
     </row>
@@ -3743,16 +3794,16 @@
         <v>118</v>
       </c>
       <c r="B123" s="3">
-        <v>77839</v>
+        <v>77761</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E123" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F123" s="3"/>
     </row>
@@ -3761,16 +3812,16 @@
         <v>119</v>
       </c>
       <c r="B124" s="3">
-        <v>77840</v>
+        <v>77766</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E124" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F124" s="3"/>
     </row>
@@ -3779,16 +3830,16 @@
         <v>120</v>
       </c>
       <c r="B125" s="3">
-        <v>77841</v>
+        <v>77770</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E125" s="3">
-        <v>13896</v>
+        <v>13893</v>
       </c>
       <c r="F125" s="3"/>
     </row>
@@ -3796,17 +3847,17 @@
       <c r="A126" s="2">
         <v>121</v>
       </c>
-      <c r="B126" s="6">
-        <v>77845</v>
+      <c r="B126" s="3">
+        <v>77777</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="E126" s="3">
-        <v>13909</v>
+        <v>13893</v>
       </c>
       <c r="F126" s="3"/>
     </row>
@@ -3815,10 +3866,10 @@
         <v>122</v>
       </c>
       <c r="B127" s="3">
-        <v>77846</v>
+        <v>77778</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>55</v>
@@ -3832,17 +3883,17 @@
       <c r="A128" s="2">
         <v>123</v>
       </c>
-      <c r="B128" s="2">
-        <v>77847</v>
+      <c r="B128" s="3">
+        <v>77780</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E128" s="3">
-        <v>13894</v>
+        <v>13896</v>
       </c>
       <c r="F128" s="3"/>
     </row>
@@ -3851,16 +3902,16 @@
         <v>124</v>
       </c>
       <c r="B129" s="3">
-        <v>77869</v>
+        <v>77781</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E129" s="3">
-        <v>13901</v>
+        <v>13896</v>
       </c>
       <c r="F129" s="3"/>
     </row>
@@ -3869,16 +3920,16 @@
         <v>125</v>
       </c>
       <c r="B130" s="3">
-        <v>77870</v>
+        <v>77782</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E130" s="3">
-        <v>13901</v>
+        <v>13896</v>
       </c>
       <c r="F130" s="3"/>
     </row>
@@ -3886,17 +3937,17 @@
       <c r="A131" s="2">
         <v>126</v>
       </c>
-      <c r="B131" s="6">
-        <v>77871</v>
-      </c>
-      <c r="C131" s="7" t="s">
-        <v>80</v>
+      <c r="B131" s="3">
+        <v>77834</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E131" s="3">
-        <v>13901</v>
+        <v>13896</v>
       </c>
       <c r="F131" s="3"/>
     </row>
@@ -3904,17 +3955,17 @@
       <c r="A132" s="2">
         <v>127</v>
       </c>
-      <c r="B132" s="6">
-        <v>77872</v>
+      <c r="B132" s="4">
+        <v>77835</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E132" s="3">
-        <v>13901</v>
+        <v>13896</v>
       </c>
       <c r="F132" s="3"/>
     </row>
@@ -3922,17 +3973,17 @@
       <c r="A133" s="2">
         <v>128</v>
       </c>
-      <c r="B133" s="6">
-        <v>77873</v>
+      <c r="B133" s="3">
+        <v>77836</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E133" s="3">
-        <v>13901</v>
+        <v>13896</v>
       </c>
       <c r="F133" s="3"/>
     </row>
@@ -3941,16 +3992,16 @@
         <v>129</v>
       </c>
       <c r="B134" s="3">
-        <v>77874</v>
+        <v>77839</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>176</v>
+        <v>55</v>
       </c>
       <c r="E134" s="3">
-        <v>13903</v>
+        <v>13896</v>
       </c>
       <c r="F134" s="3"/>
     </row>
@@ -3958,17 +4009,17 @@
       <c r="A135" s="2">
         <v>130</v>
       </c>
-      <c r="B135" s="2">
-        <v>77876</v>
+      <c r="B135" s="3">
+        <v>77840</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E135" s="3">
-        <v>13894</v>
+        <v>13896</v>
       </c>
       <c r="F135" s="3"/>
     </row>
@@ -3976,17 +4027,17 @@
       <c r="A136" s="2">
         <v>131</v>
       </c>
-      <c r="B136" s="2">
-        <v>81032</v>
+      <c r="B136" s="3">
+        <v>77841</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>179</v>
+        <v>55</v>
       </c>
       <c r="E136" s="3">
-        <v>11069</v>
+        <v>13896</v>
       </c>
       <c r="F136" s="3"/>
     </row>
@@ -3994,17 +4045,17 @@
       <c r="A137" s="2">
         <v>132</v>
       </c>
-      <c r="B137" s="2">
-        <v>81043</v>
+      <c r="B137" s="4">
+        <v>77845</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="E137" s="3">
-        <v>11070</v>
+        <v>13909</v>
       </c>
       <c r="F137" s="3"/>
     </row>
@@ -4012,17 +4063,17 @@
       <c r="A138" s="2">
         <v>133</v>
       </c>
-      <c r="B138" s="2">
-        <v>96726</v>
+      <c r="B138" s="3">
+        <v>77846</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E138" s="3">
-        <v>12588</v>
+        <v>13896</v>
       </c>
       <c r="F138" s="3"/>
     </row>
@@ -4031,16 +4082,16 @@
         <v>134</v>
       </c>
       <c r="B139" s="2">
-        <v>96727</v>
+        <v>77847</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>184</v>
+        <v>44</v>
       </c>
       <c r="E139" s="3">
-        <v>12589</v>
+        <v>13894</v>
       </c>
       <c r="F139" s="3"/>
     </row>
@@ -4048,17 +4099,17 @@
       <c r="A140" s="2">
         <v>135</v>
       </c>
-      <c r="B140" s="2">
-        <v>96728</v>
+      <c r="B140" s="3">
+        <v>77869</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="E140" s="3">
-        <v>12590</v>
+        <v>13901</v>
       </c>
       <c r="F140" s="3"/>
     </row>
@@ -4066,17 +4117,17 @@
       <c r="A141" s="2">
         <v>136</v>
       </c>
-      <c r="B141" s="2">
-        <v>96729</v>
+      <c r="B141" s="3">
+        <v>77870</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>187</v>
+        <v>80</v>
       </c>
       <c r="E141" s="3">
-        <v>12591</v>
+        <v>13901</v>
       </c>
       <c r="F141" s="3"/>
     </row>
@@ -4084,17 +4135,17 @@
       <c r="A142" s="2">
         <v>137</v>
       </c>
-      <c r="B142" s="2">
-        <v>96730</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>188</v>
+      <c r="B142" s="4">
+        <v>77871</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="E142" s="3">
-        <v>12592</v>
+        <v>13901</v>
       </c>
       <c r="F142" s="3"/>
     </row>
@@ -4102,17 +4153,17 @@
       <c r="A143" s="2">
         <v>138</v>
       </c>
-      <c r="B143" s="2">
-        <v>96731</v>
+      <c r="B143" s="4">
+        <v>77872</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>190</v>
+        <v>80</v>
       </c>
       <c r="E143" s="3">
-        <v>12593</v>
+        <v>13901</v>
       </c>
       <c r="F143" s="3"/>
     </row>
@@ -4120,17 +4171,17 @@
       <c r="A144" s="2">
         <v>139</v>
       </c>
-      <c r="B144" s="6">
-        <v>96732</v>
+      <c r="B144" s="4">
+        <v>77873</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E144" s="3">
-        <v>13899</v>
+        <v>13901</v>
       </c>
       <c r="F144" s="3"/>
     </row>
@@ -4138,17 +4189,17 @@
       <c r="A145" s="2">
         <v>140</v>
       </c>
-      <c r="B145" s="6">
-        <v>98933</v>
+      <c r="B145" s="3">
+        <v>77874</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="E145" s="3">
-        <v>13899</v>
+        <v>13903</v>
       </c>
       <c r="F145" s="3"/>
     </row>
@@ -4156,17 +4207,17 @@
       <c r="A146" s="2">
         <v>141</v>
       </c>
-      <c r="B146" s="6">
-        <v>98934</v>
+      <c r="B146" s="2">
+        <v>77876</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E146" s="3">
-        <v>13899</v>
+        <v>13894</v>
       </c>
       <c r="F146" s="3"/>
     </row>
@@ -4174,17 +4225,17 @@
       <c r="A147" s="2">
         <v>142</v>
       </c>
-      <c r="B147" s="6">
-        <v>98935</v>
+      <c r="B147" s="2">
+        <v>81032</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
       <c r="E147" s="3">
-        <v>13904</v>
+        <v>11069</v>
       </c>
       <c r="F147" s="3"/>
     </row>
@@ -4192,17 +4243,17 @@
       <c r="A148" s="2">
         <v>143</v>
       </c>
-      <c r="B148" s="6">
-        <v>98936</v>
+      <c r="B148" s="2">
+        <v>81043</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="E148" s="3">
-        <v>13904</v>
+        <v>11070</v>
       </c>
       <c r="F148" s="3"/>
     </row>
@@ -4210,17 +4261,17 @@
       <c r="A149" s="2">
         <v>144</v>
       </c>
-      <c r="B149" s="6">
-        <v>98937</v>
+      <c r="B149" s="2">
+        <v>96726</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E149" s="3">
-        <v>13904</v>
+        <v>12588</v>
       </c>
       <c r="F149" s="3"/>
     </row>
@@ -4228,17 +4279,17 @@
       <c r="A150" s="2">
         <v>145</v>
       </c>
-      <c r="B150" s="6">
-        <v>98938</v>
+      <c r="B150" s="2">
+        <v>96727</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="E150" s="3">
-        <v>13904</v>
+        <v>12589</v>
       </c>
       <c r="F150" s="3"/>
     </row>
@@ -4246,17 +4297,17 @@
       <c r="A151" s="2">
         <v>146</v>
       </c>
-      <c r="B151" s="6">
-        <v>98939</v>
+      <c r="B151" s="2">
+        <v>96728</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E151" s="3">
-        <v>13899</v>
+        <v>12590</v>
       </c>
       <c r="F151" s="3"/>
     </row>
@@ -4264,17 +4315,17 @@
       <c r="A152" s="2">
         <v>147</v>
       </c>
-      <c r="B152" s="6">
-        <v>98940</v>
+      <c r="B152" s="2">
+        <v>96729</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>69</v>
+        <v>187</v>
       </c>
       <c r="E152" s="3">
-        <v>13899</v>
+        <v>12591</v>
       </c>
       <c r="F152" s="3"/>
     </row>
@@ -4282,17 +4333,17 @@
       <c r="A153" s="2">
         <v>148</v>
       </c>
-      <c r="B153" s="6">
-        <v>98941</v>
+      <c r="B153" s="2">
+        <v>96730</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="E153" s="3">
-        <v>13899</v>
+        <v>12592</v>
       </c>
       <c r="F153" s="3"/>
     </row>
@@ -4300,17 +4351,17 @@
       <c r="A154" s="2">
         <v>149</v>
       </c>
-      <c r="B154" s="6">
-        <v>98942</v>
+      <c r="B154" s="2">
+        <v>96731</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>69</v>
+        <v>190</v>
       </c>
       <c r="E154" s="3">
-        <v>13899</v>
+        <v>12593</v>
       </c>
       <c r="F154" s="3"/>
     </row>
@@ -4318,17 +4369,17 @@
       <c r="A155" s="2">
         <v>150</v>
       </c>
-      <c r="B155" s="6">
-        <v>98943</v>
+      <c r="B155" s="4">
+        <v>96732</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="E155" s="3">
-        <v>13905</v>
+        <v>13899</v>
       </c>
       <c r="F155" s="3"/>
     </row>
@@ -4336,17 +4387,17 @@
       <c r="A156" s="2">
         <v>151</v>
       </c>
-      <c r="B156" s="6">
-        <v>98944</v>
+      <c r="B156" s="4">
+        <v>98933</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="E156" s="3">
-        <v>13905</v>
+        <v>13899</v>
       </c>
       <c r="F156" s="3"/>
     </row>
@@ -4354,17 +4405,17 @@
       <c r="A157" s="2">
         <v>152</v>
       </c>
-      <c r="B157" s="6">
-        <v>98945</v>
+      <c r="B157" s="4">
+        <v>98934</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="E157" s="3">
-        <v>13905</v>
+        <v>13899</v>
       </c>
       <c r="F157" s="3"/>
     </row>
@@ -4372,17 +4423,17 @@
       <c r="A158" s="2">
         <v>153</v>
       </c>
-      <c r="B158" s="6">
-        <v>98946</v>
+      <c r="B158" s="4">
+        <v>98935</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="E158" s="3">
-        <v>13899</v>
+        <v>13904</v>
       </c>
       <c r="F158" s="3"/>
     </row>
@@ -4390,17 +4441,17 @@
       <c r="A159" s="2">
         <v>154</v>
       </c>
-      <c r="B159" s="6">
-        <v>98948</v>
+      <c r="B159" s="4">
+        <v>98936</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="E159" s="3">
-        <v>13905</v>
+        <v>13904</v>
       </c>
       <c r="F159" s="3"/>
     </row>
@@ -4408,17 +4459,17 @@
       <c r="A160" s="2">
         <v>155</v>
       </c>
-      <c r="B160" s="2">
-        <v>98949</v>
+      <c r="B160" s="4">
+        <v>98937</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E160" s="3">
-        <v>13895</v>
+        <v>13904</v>
       </c>
       <c r="F160" s="3"/>
     </row>
@@ -4426,17 +4477,17 @@
       <c r="A161" s="2">
         <v>156</v>
       </c>
-      <c r="B161" s="6">
-        <v>98950</v>
+      <c r="B161" s="4">
+        <v>98938</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>210</v>
+        <v>38</v>
       </c>
       <c r="E161" s="3">
-        <v>13906</v>
+        <v>13904</v>
       </c>
       <c r="F161" s="3"/>
     </row>
@@ -4444,17 +4495,17 @@
       <c r="A162" s="2">
         <v>157</v>
       </c>
-      <c r="B162" s="2">
-        <v>98951</v>
+      <c r="B162" s="4">
+        <v>98939</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="E162" s="3">
-        <v>13894</v>
+        <v>13899</v>
       </c>
       <c r="F162" s="3"/>
     </row>
@@ -4462,17 +4513,17 @@
       <c r="A163" s="2">
         <v>158</v>
       </c>
-      <c r="B163" s="2">
-        <v>98952</v>
+      <c r="B163" s="4">
+        <v>98940</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="E163" s="3">
-        <v>13894</v>
+        <v>13899</v>
       </c>
       <c r="F163" s="3"/>
     </row>
@@ -4480,17 +4531,17 @@
       <c r="A164" s="2">
         <v>159</v>
       </c>
-      <c r="B164" s="6">
-        <v>98953</v>
+      <c r="B164" s="4">
+        <v>98941</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>214</v>
+        <v>69</v>
       </c>
       <c r="E164" s="3">
-        <v>13907</v>
+        <v>13899</v>
       </c>
       <c r="F164" s="3"/>
     </row>
@@ -4498,17 +4549,17 @@
       <c r="A165" s="2">
         <v>160</v>
       </c>
-      <c r="B165" s="6">
-        <v>98987</v>
+      <c r="B165" s="4">
+        <v>98942</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>216</v>
+        <v>69</v>
       </c>
       <c r="E165" s="3">
-        <v>13688</v>
+        <v>13899</v>
       </c>
       <c r="F165" s="3"/>
     </row>
@@ -4516,17 +4567,17 @@
       <c r="A166" s="2">
         <v>161</v>
       </c>
-      <c r="B166" s="2">
-        <v>99010</v>
+      <c r="B166" s="4">
+        <v>98943</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="E166" s="3">
-        <v>12594</v>
+        <v>13905</v>
       </c>
       <c r="F166" s="3"/>
     </row>
@@ -4534,31 +4585,35 @@
       <c r="A167" s="2">
         <v>162</v>
       </c>
-      <c r="B167" s="6">
-        <v>105396</v>
+      <c r="B167" s="4">
+        <v>98944</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D167" s="3"/>
-      <c r="E167" s="3"/>
+        <v>202</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E167" s="3">
+        <v>13905</v>
+      </c>
       <c r="F167" s="3"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>163</v>
       </c>
-      <c r="B168" s="6">
-        <v>105932</v>
+      <c r="B168" s="4">
+        <v>98945</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="E168" s="3">
-        <v>13908</v>
+        <v>13905</v>
       </c>
       <c r="F168" s="3"/>
     </row>
@@ -4566,17 +4621,17 @@
       <c r="A169" s="2">
         <v>164</v>
       </c>
-      <c r="B169" s="3">
-        <v>105933</v>
+      <c r="B169" s="4">
+        <v>98946</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="E169" s="3">
-        <v>13894</v>
+        <v>13899</v>
       </c>
       <c r="F169" s="3"/>
     </row>
@@ -4584,22 +4639,216 @@
       <c r="A170" s="2">
         <v>165</v>
       </c>
-      <c r="B170" s="6">
+      <c r="B170" s="4">
+        <v>98948</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E170" s="3">
+        <v>13905</v>
+      </c>
+      <c r="F170" s="3"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>166</v>
+      </c>
+      <c r="B171" s="2">
+        <v>98949</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E171" s="3">
+        <v>13895</v>
+      </c>
+      <c r="F171" s="3"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>167</v>
+      </c>
+      <c r="B172" s="4">
+        <v>98950</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E172" s="3">
+        <v>13906</v>
+      </c>
+      <c r="F172" s="3"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>168</v>
+      </c>
+      <c r="B173" s="2">
+        <v>98951</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E173" s="3">
+        <v>13894</v>
+      </c>
+      <c r="F173" s="3"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>169</v>
+      </c>
+      <c r="B174" s="2">
+        <v>98952</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E174" s="3">
+        <v>13894</v>
+      </c>
+      <c r="F174" s="3"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>170</v>
+      </c>
+      <c r="B175" s="4">
+        <v>98953</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E175" s="3">
+        <v>13907</v>
+      </c>
+      <c r="F175" s="3"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>171</v>
+      </c>
+      <c r="B176" s="4">
+        <v>98987</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E176" s="3">
+        <v>13688</v>
+      </c>
+      <c r="F176" s="3"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>172</v>
+      </c>
+      <c r="B177" s="2">
+        <v>99010</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E177" s="3">
+        <v>12594</v>
+      </c>
+      <c r="F177" s="3"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>173</v>
+      </c>
+      <c r="B178" s="4">
+        <v>105396</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D178" s="3"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>174</v>
+      </c>
+      <c r="B179" s="4">
+        <v>105932</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E179" s="3">
+        <v>13908</v>
+      </c>
+      <c r="F179" s="3"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>175</v>
+      </c>
+      <c r="B180" s="3">
+        <v>105933</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E180" s="3">
+        <v>13894</v>
+      </c>
+      <c r="F180" s="3"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>176</v>
+      </c>
+      <c r="B181" s="4">
         <v>105934</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C181" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D181" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E170" s="3">
+      <c r="E181" s="3">
         <v>13898</v>
       </c>
-      <c r="F170" s="3"/>
+      <c r="F181" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="B6:B171">
+  <sortState ref="B6:E181">
     <sortCondition ref="B6"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>